<commit_message>
Test different types of emotions
</commit_message>
<xml_diff>
--- a/EmotionRegulation/EmotionRegulationAsset/Results/Conscientiousness.xlsx
+++ b/EmotionRegulation/EmotionRegulationAsset/Results/Conscientiousness.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R3beb2c02d24545ec"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="Rf5b02a8f98d34477"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <x:si>
     <x:t xml:space="preserve">MOOD     </x:t>
   </x:si>
@@ -92,10 +92,16 @@
     <x:t>Fly</x:t>
   </x:si>
   <x:si>
+    <x:t>Gloating</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BecomeRich</x:t>
+  </x:si>
+  <x:si>
     <x:t>High Conscientiousness</x:t>
   </x:si>
   <x:si>
-    <x:t>Low Extraversion</x:t>
+    <x:t>Middle Extraversion</x:t>
   </x:si>
   <x:si>
     <x:t>Low Neuroticism</x:t>
@@ -450,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:H44"/>
+  <x:dimension ref="A1:H23"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -484,13 +490,13 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>-0.9341458082199097</x:v>
+        <x:v>-0.7233197093009949</x:v>
       </x:c>
       <x:c r="B2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>3.007751226425171</x:v>
+        <x:v>2.3289358615875244</x:v>
       </x:c>
       <x:c r="D2" t="s">
         <x:v>9</x:v>
@@ -507,7 +513,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>1.7375788688659668</x:v>
+        <x:v>1.7979705333709717</x:v>
       </x:c>
       <x:c r="D3" t="s">
         <x:v>12</x:v>
@@ -552,13 +558,13 @@
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>1.614364743232727</x:v>
+        <x:v>1.8665099143981934</x:v>
       </x:c>
       <x:c r="B6" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>2.274688959121704</x:v>
+        <x:v>1.462835431098938</x:v>
       </x:c>
       <x:c r="D6" t="s">
         <x:v>16</x:v>
@@ -569,13 +575,13 @@
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>2.332554578781128</x:v>
+        <x:v>2.604235887527466</x:v>
       </x:c>
       <x:c r="B7" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>2.372122049331665</x:v>
+        <x:v>2.444349527359009</x:v>
       </x:c>
       <x:c r="D7" t="s">
         <x:v>18</x:v>
@@ -586,13 +592,13 @@
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>1.5978124141693115</x:v>
+        <x:v>2.1493771076202393</x:v>
       </x:c>
       <x:c r="B8" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>2.2794501781463623</x:v>
+        <x:v>1.368237853050232</x:v>
       </x:c>
       <x:c r="D8" t="s">
         <x:v>19</x:v>
@@ -603,13 +609,13 @@
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>0.71785569190979</x:v>
+        <x:v>1.5964168310165405</x:v>
       </x:c>
       <x:c r="B9" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>2.5780723094940186</x:v>
+        <x:v>1.7009257078170776</x:v>
       </x:c>
       <x:c r="D9" t="s">
         <x:v>21</x:v>
@@ -620,13 +626,13 @@
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>0</x:v>
+        <x:v>1.0882270336151123</x:v>
       </x:c>
       <x:c r="B10" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>2.895329236984253</x:v>
+        <x:v>2.0543439388275146</x:v>
       </x:c>
       <x:c r="D10" t="s">
         <x:v>22</x:v>
@@ -637,13 +643,13 @@
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>2.372433662414551</x:v>
+        <x:v>3.5449769496917725</x:v>
       </x:c>
       <x:c r="B11" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>7.63873291015625</x:v>
+        <x:v>7.950458526611328</x:v>
       </x:c>
       <x:c r="D11" t="s">
         <x:v>23</x:v>
@@ -654,13 +660,13 @@
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>1.6144108772277832</x:v>
+        <x:v>3.1017425060272217</x:v>
       </x:c>
       <x:c r="B12" t="s">
         <x:v>24</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>2.3529343605041504</x:v>
+        <x:v>1.2960190773010254</x:v>
       </x:c>
       <x:c r="D12" t="s">
         <x:v>25</x:v>
@@ -671,426 +677,69 @@
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>0.5384464263916016</x:v>
+        <x:v>3.9741029739379883</x:v>
       </x:c>
       <x:c r="B13" t="s">
-        <x:v>8</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>2.5780723094940186</x:v>
+        <x:v>2.923525094985962</x:v>
       </x:c>
       <x:c r="D13" t="s">
-        <x:v>9</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E13" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
-      <x:c r="A14">
-        <x:v>1.202929139137268</x:v>
-      </x:c>
-      <x:c r="B14" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C14">
-        <x:v>2.1594064235687256</x:v>
-      </x:c>
-      <x:c r="D14" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E14" t="s">
-        <x:v>13</x:v>
+      <x:c r="F14" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
-      <x:c r="A15">
-        <x:v>2.1264841556549072</x:v>
-      </x:c>
-      <x:c r="B15" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C15">
-        <x:v>3.0181384086608887</x:v>
-      </x:c>
-      <x:c r="D15" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E15" t="s">
-        <x:v>13</x:v>
+      <x:c r="F15" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
-      <x:c r="A16">
-        <x:v>3.7443604469299316</x:v>
-      </x:c>
-      <x:c r="B16" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C16">
-        <x:v>5.28786039352417</x:v>
-      </x:c>
-      <x:c r="D16" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E16" t="s">
-        <x:v>13</x:v>
+      <x:c r="F16" t="s">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
-      <x:c r="A17">
-        <x:v>3.130309820175171</x:v>
-      </x:c>
-      <x:c r="B17" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C17">
-        <x:v>1.8386374711990356</x:v>
-      </x:c>
-      <x:c r="D17" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="E17" t="s">
-        <x:v>10</x:v>
+      <x:c r="F17" t="s">
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
-      <x:c r="A18">
-        <x:v>3.9659554958343506</x:v>
-      </x:c>
-      <x:c r="B18" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C18">
-        <x:v>2.806368350982666</x:v>
-      </x:c>
-      <x:c r="D18" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E18" t="s">
-        <x:v>13</x:v>
+      <x:c r="F18" t="s">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
-      <x:c r="A19">
-        <x:v>3.3708481788635254</x:v>
-      </x:c>
-      <x:c r="B19" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C19">
-        <x:v>1.7694480419158936</x:v>
-      </x:c>
-      <x:c r="D19" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E19" t="s">
-        <x:v>10</x:v>
+      <x:c r="G19" t="s">
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
-      <x:c r="A20">
-        <x:v>2.708853006362915</x:v>
-      </x:c>
-      <x:c r="B20" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C20">
-        <x:v>2.006821870803833</x:v>
-      </x:c>
-      <x:c r="D20" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E20" t="s">
-        <x:v>10</x:v>
+      <x:c r="G20" t="s">
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
-      <x:c r="A21">
-        <x:v>1.9715827703475952</x:v>
-      </x:c>
-      <x:c r="B21" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C21">
-        <x:v>2.2736737728118896</x:v>
-      </x:c>
-      <x:c r="D21" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E21" t="s">
-        <x:v>10</x:v>
+      <x:c r="G21" t="s">
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="22">
-      <x:c r="A22">
-        <x:v>4.496775150299072</x:v>
-      </x:c>
-      <x:c r="B22" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C22">
-        <x:v>8.203496932983398</x:v>
-      </x:c>
-      <x:c r="D22" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E22" t="s">
-        <x:v>13</x:v>
+      <x:c r="G22" t="s">
+        <x:v>36</x:v>
       </x:c>
     </x:row>
     <x:row r="23">
-      <x:c r="A23">
-        <x:v>3.920356512069702</x:v>
-      </x:c>
-      <x:c r="B23" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C23">
-        <x:v>1.6896443367004395</x:v>
-      </x:c>
-      <x:c r="D23" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E23" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24">
-      <x:c r="A24">
-        <x:v>3.3213510513305664</x:v>
-      </x:c>
-      <x:c r="B24" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C24">
-        <x:v>1.783685564994812</x:v>
-      </x:c>
-      <x:c r="D24" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E24" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25">
-      <x:c r="A25">
-        <x:v>4.201454162597656</x:v>
-      </x:c>
-      <x:c r="B25" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C25">
-        <x:v>2.9565765857696533</x:v>
-      </x:c>
-      <x:c r="D25" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E25" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26">
-      <x:c r="A26">
-        <x:v>5.357336044311523</x:v>
-      </x:c>
-      <x:c r="B26" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C26">
-        <x:v>3.8770735263824463</x:v>
-      </x:c>
-      <x:c r="D26" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="E26" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27">
-      <x:c r="A27">
-        <x:v>7.225539684295654</x:v>
-      </x:c>
-      <x:c r="B27" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C27">
-        <x:v>6.213346481323242</x:v>
-      </x:c>
-      <x:c r="D27" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="E27" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28">
-      <x:c r="A28">
-        <x:v>6.302605628967285</x:v>
-      </x:c>
-      <x:c r="B28" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C28">
-        <x:v>2.704434394836426</x:v>
-      </x:c>
-      <x:c r="D28" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="E28" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29">
-      <x:c r="A29">
-        <x:v>7.384041786193848</x:v>
-      </x:c>
-      <x:c r="B29" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C29">
-        <x:v>3.715080499649048</x:v>
-      </x:c>
-      <x:c r="D29" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="E29" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30">
-      <x:c r="A30">
-        <x:v>6.473388195037842</x:v>
-      </x:c>
-      <x:c r="B30" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="C30">
-        <x:v>2.6590309143066406</x:v>
-      </x:c>
-      <x:c r="D30" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E30" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31">
-      <x:c r="A31">
-        <x:v>6.076621055603027</x:v>
-      </x:c>
-      <x:c r="B31" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C31">
-        <x:v>1.0381057262420654</x:v>
-      </x:c>
-      <x:c r="D31" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="E31" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32">
-      <x:c r="A32">
-        <x:v>5.627252101898193</x:v>
-      </x:c>
-      <x:c r="B32" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C32">
-        <x:v>1.2221447229385376</x:v>
-      </x:c>
-      <x:c r="D32" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E32" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33">
-      <x:c r="A33">
-        <x:v>8.435687065124512</x:v>
-      </x:c>
-      <x:c r="B33" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C33">
-        <x:v>9.250673294067383</x:v>
-      </x:c>
-      <x:c r="D33" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="E33" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34">
-      <x:c r="A34">
-        <x:v>8.042240142822266</x:v>
-      </x:c>
-      <x:c r="B34" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C34">
-        <x:v>0.9548416137695312</x:v>
-      </x:c>
-      <x:c r="D34" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="E34" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35">
-      <x:c r="F35" t="s">
-        <x:v>26</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36">
-      <x:c r="F36" t="s">
-        <x:v>27</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37">
-      <x:c r="F37" t="s">
-        <x:v>28</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38">
-      <x:c r="F38" t="s">
-        <x:v>29</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="39">
-      <x:c r="F39" t="s">
-        <x:v>30</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40">
-      <x:c r="G40" t="s">
-        <x:v>31</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41">
-      <x:c r="G41" t="s">
-        <x:v>32</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="42">
-      <x:c r="G42" t="s">
-        <x:v>33</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43">
-      <x:c r="G43" t="s">
-        <x:v>34</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44">
-      <x:c r="H44" t="s">
-        <x:v>35</x:v>
+      <x:c r="H23" t="s">
+        <x:v>37</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>